<commit_message>
add feature to word count script
</commit_message>
<xml_diff>
--- a/examples/greetings.xlsx
+++ b/examples/greetings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox (Personal)\Code\excel2csv\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD89D06-0463-45BD-98F4-41425F567E32}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9BB82CE-971A-41A3-9489-AD1BBFA287DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="34400" windowHeight="17730" activeTab="1" xr2:uid="{F687CA4F-F0FB-4BA6-B7E1-15AC6AF9BDF1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="34400" windowHeight="17730" xr2:uid="{F687CA4F-F0FB-4BA6-B7E1-15AC6AF9BDF1}"/>
   </bookViews>
   <sheets>
     <sheet name="GREETINGS" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t>#Date</t>
   </si>
@@ -107,6 +107,24 @@
   </si>
   <si>
     <t>Using an Excel spreadsheet like this lets you add useful comments.</t>
+  </si>
+  <si>
+    <t>GREETING_4</t>
+  </si>
+  <si>
+    <t>Howdy.</t>
+  </si>
+  <si>
+    <t>Not translated yet, so don't include in word count.</t>
+  </si>
+  <si>
+    <t>GREETING_5</t>
+  </si>
+  <si>
+    <t>HELLO!</t>
+  </si>
+  <si>
+    <t>Same content, so don't include in word count.</t>
   </si>
 </sst>
 </file>
@@ -459,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78E0ABA6-A3EA-4139-8BB4-D6B714CD5D8D}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -550,6 +568,43 @@
         <v>26</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>44021</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>44021</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -559,7 +614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74A3974B-B731-4350-9BA9-B312B3E2ECA8}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add example about how to use replace command
</commit_message>
<xml_diff>
--- a/examples/greetings.xlsx
+++ b/examples/greetings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MaxUser\Projects\excel2csv\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C334FE3-3370-4788-ABC7-7FA148C389A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D18D49-3620-4997-9F77-CE32F1D38A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{F687CA4F-F0FB-4BA6-B7E1-15AC6AF9BDF1}"/>
+    <workbookView xWindow="1160" yWindow="2840" windowWidth="28710" windowHeight="15340" xr2:uid="{F687CA4F-F0FB-4BA6-B7E1-15AC6AF9BDF1}"/>
   </bookViews>
   <sheets>
     <sheet name="GREETINGS" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -112,9 +123,6 @@
     <t>GREETING_4</t>
   </si>
   <si>
-    <t>Howdy.</t>
-  </si>
-  <si>
     <t>Not translated yet, so don't include in word count.</t>
   </si>
   <si>
@@ -142,6 +150,9 @@
   </si>
   <si>
     <t>Newline should be replaced.</t>
+  </si>
+  <si>
+    <t>Howdy…</t>
   </si>
 </sst>
 </file>
@@ -501,7 +512,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -600,10 +611,10 @@
         <v>27</v>
       </c>
       <c r="D5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" t="s">
         <v>28</v>
-      </c>
-      <c r="F5" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -614,16 +625,16 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
         <v>30</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
         <v>31</v>
-      </c>
-      <c r="E6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -634,7 +645,7 @@
         <v>5</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -645,16 +656,16 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="F8" t="s">
         <v>36</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>